<commit_message>
Minor updates to dataset
</commit_message>
<xml_diff>
--- a/dog_data.xlsx
+++ b/dog_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TEKNOJOES TEKNOTOOL\Desktop\projects\Data-Cleaning-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6721058C-2FC4-4321-AE8D-DA5A523A664A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38704E23-7B3E-4490-AA7C-ACA15DB953F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5355" yWindow="5505" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6225" yWindow="5910" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Doggy daycare member list" sheetId="1" r:id="rId1"/>
@@ -129,9 +129,6 @@
     <t>Tiny</t>
   </si>
   <si>
-    <t>Cozzy</t>
-  </si>
-  <si>
     <t>Shelina</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>Cozy</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -567,7 +567,7 @@
         <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
@@ -733,10 +733,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -748,18 +748,18 @@
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>

</xml_diff>